<commit_message>
Technical Report added.  README.md edited. EDA work
</commit_message>
<xml_diff>
--- a/Capstone Data Dictionary - GOAT Talk.xlsx
+++ b/Capstone Data Dictionary - GOAT Talk.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/omarcarr/Desktop/Notebooks/DSI-US-5/Capstone-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{794F8F1D-AA02-2244-A7A1-1CB21C078D93}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C11F05AE-FA77-064E-A6A5-22E4E1F07EA8}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="680" windowWidth="22820" windowHeight="17440" xr2:uid="{E3754559-B868-A345-A4EC-ADD2D0881418}"/>
+    <workbookView xWindow="80" yWindow="7840" windowWidth="18060" windowHeight="15140" xr2:uid="{E3754559-B868-A345-A4EC-ADD2D0881418}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="86">
   <si>
     <t>Data Dictionary</t>
   </si>
@@ -150,13 +145,151 @@
   </si>
   <si>
     <t>Average Number of Offensive Rebounds Per Game (Player's team on offense and he gains rebound off of teammates' shot to give them another possession)</t>
+  </si>
+  <si>
+    <t>Defensive Reb Per Game</t>
+  </si>
+  <si>
+    <t>Average Number of Defensive Rebounds Per Game (Player's team on defense and he gains rebound off of opponent's shot to giv ethem possession</t>
+  </si>
+  <si>
+    <t>Total Reb Per Game</t>
+  </si>
+  <si>
+    <t>Average Number of Total (Offensive and Defensive) Rebounds Per Game</t>
+  </si>
+  <si>
+    <t>Assists Per Game</t>
+  </si>
+  <si>
+    <t>Average Number of Assists Per Game</t>
+  </si>
+  <si>
+    <t>Steals Per Game</t>
+  </si>
+  <si>
+    <t>Average Number of Steals Per Game</t>
+  </si>
+  <si>
+    <t>Blocks Per Game</t>
+  </si>
+  <si>
+    <t>Turnovers Per Game</t>
+  </si>
+  <si>
+    <t>Fouls Per Game</t>
+  </si>
+  <si>
+    <t>Points Per Game</t>
+  </si>
+  <si>
+    <t>Average Number of Blocks Per Game</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Average Number of Turnovers Per Game </t>
+  </si>
+  <si>
+    <t>Average Number of Personal Fouls Per Game (Different from Technical Fouls)</t>
+  </si>
+  <si>
+    <t>Average Number of Points Per Game</t>
+  </si>
+  <si>
+    <t>Per Game Statistics</t>
+  </si>
+  <si>
+    <t>Advanced Statistics</t>
+  </si>
+  <si>
+    <t>PER (Player Efficiency Rating)</t>
+  </si>
+  <si>
+    <t>A measure of per-minute production; league average is 15</t>
+  </si>
+  <si>
+    <t>TS% (True Shooting %)</t>
+  </si>
+  <si>
+    <t>A measure of shooting efficiency that takes into account 2-point FGs, 3-point FGs, and FT</t>
+  </si>
+  <si>
+    <t>TRB% (Total Rebound %)</t>
+  </si>
+  <si>
+    <t>An estimate of the percentage of available rebounds a player grabbed while he was on the floor</t>
+  </si>
+  <si>
+    <t>Assist %</t>
+  </si>
+  <si>
+    <t>An estimate of the percentage of teammage FGs a player assisted while he was on the floor</t>
+  </si>
+  <si>
+    <t>Steal %</t>
+  </si>
+  <si>
+    <t>An estimate of the percentage of opponent possessions that end with a steal by the player while he was on the floor</t>
+  </si>
+  <si>
+    <t>Block %</t>
+  </si>
+  <si>
+    <t>An estimate of the percentage of opponent 2-point FG attempts blocked by the player while he was on the floor</t>
+  </si>
+  <si>
+    <t>TOV % (Turnover %)</t>
+  </si>
+  <si>
+    <t>An estimate of turnovers committed per 100 plays</t>
+  </si>
+  <si>
+    <t>Usage %</t>
+  </si>
+  <si>
+    <t>An estimate of the percentage of team plays used by a player while he was on the floor</t>
+  </si>
+  <si>
+    <t>WS (Win Shares)</t>
+  </si>
+  <si>
+    <t>An estimate of the number of wins contributed by a player</t>
+  </si>
+  <si>
+    <t>OBPM (Offensive Box Plus/Minus)</t>
+  </si>
+  <si>
+    <t>A box score estimate of the offensive points per 100 possessions a player contributed above a league-average player, translated to an average team</t>
+  </si>
+  <si>
+    <t>DBPM (Defensive Box Plus/Minus</t>
+  </si>
+  <si>
+    <t>A box score estimate of the defensive points per 100 possessions a player contributed above a league-average player, translated to an average team</t>
+  </si>
+  <si>
+    <t>BPM (Box Plus/Minus)</t>
+  </si>
+  <si>
+    <t>A box score estimate of the points per 100 possessions a player contributed above a league-average player, translated to an average team</t>
+  </si>
+  <si>
+    <t>A box score estimate of the points per 100 TEAM possessions that a player contributed above a replacement-level (-2.0) player, translated to an average team and prorated to an 82-game season</t>
+  </si>
+  <si>
+    <t>VORP (Value over Replacement Player)</t>
+  </si>
+  <si>
+    <t>WOR (Wins over Replacement)</t>
+  </si>
+  <si>
+    <t>VORP score * 2.70</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -170,6 +303,20 @@
       <name val="Calibri Light"/>
       <family val="2"/>
       <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -192,9 +339,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -511,10 +664,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3B66892-6DCD-B54E-9BE2-A3160E7025B5}">
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -546,207 +699,475 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
         <v>28</v>
       </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B17" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
         <v>32</v>
       </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>34</v>
       </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
         <v>39</v>
       </c>
     </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>66</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>83</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:H2"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A32:H32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>